<commit_message>
clean up chart drawing functions and add to read me"
</commit_message>
<xml_diff>
--- a/sample_data/SampleData.xlsx
+++ b/sample_data/SampleData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Vicky/Documents/RChartTemplates/UHEROtheme/sample_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vicky/Documents/R/UHEROtheme/sample_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C51C602A-0ED5-8643-BB77-271E995FD4D6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16D638C4-FABF-DD4B-9FD4-06BF39F005FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6360" yWindow="1700" windowWidth="27240" windowHeight="16440" activeTab="6" xr2:uid="{37EF705C-9ABB-BC49-956B-53E83ECDB111}"/>
+    <workbookView xWindow="6360" yWindow="1700" windowWidth="27240" windowHeight="16440" activeTab="1" xr2:uid="{37EF705C-9ABB-BC49-956B-53E83ECDB111}"/>
   </bookViews>
   <sheets>
     <sheet name="Nonfarm Payrolls" sheetId="1" r:id="rId1"/>
@@ -21,10 +21,21 @@
     <sheet name="Vexp By Mkt" sheetId="6" r:id="rId6"/>
     <sheet name="Transactions" sheetId="8" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -234,18 +245,17 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4"/>
   </cellXfs>
@@ -270,9 +280,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -310,7 +320,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -416,7 +426,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -558,7 +568,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1623,8 +1633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A79EC09-1951-2A4F-9892-1CD1D59E1A18}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1790,10 +1800,10 @@
       <c r="A4" s="1">
         <v>42064</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>20.3333333333333</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>25.134666666666664</v>
       </c>
     </row>
@@ -1801,10 +1811,10 @@
       <c r="A5" s="1">
         <v>42095</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>19.333333333333332</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>24.647000000000002</v>
       </c>
     </row>
@@ -1812,10 +1822,10 @@
       <c r="A6" s="1">
         <v>42125</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>19.333333333333332</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>24.078333333333333</v>
       </c>
     </row>
@@ -1823,10 +1833,10 @@
       <c r="A7" s="1">
         <v>42156</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <v>18.333333333333332</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>23.486333333333334</v>
       </c>
     </row>
@@ -1834,10 +1844,10 @@
       <c r="A8" s="1">
         <v>42186</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="2">
         <v>19.333333333333332</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <v>22.934666666666669</v>
       </c>
     </row>
@@ -1845,10 +1855,10 @@
       <c r="A9" s="1">
         <v>42217</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="2">
         <v>19.333333333333332</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="2">
         <v>22.457333333333334</v>
       </c>
     </row>
@@ -1856,10 +1866,10 @@
       <c r="A10" s="1">
         <v>42248</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="2">
         <v>20.666666666666668</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="2">
         <v>22.049333333333333</v>
       </c>
     </row>
@@ -1867,10 +1877,10 @@
       <c r="A11" s="1">
         <v>42278</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="2">
         <v>20.333333333333332</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="2">
         <v>21.686333333333334</v>
       </c>
     </row>
@@ -1878,10 +1888,10 @@
       <c r="A12" s="1">
         <v>42309</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="2">
         <v>20.666666666666668</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="2">
         <v>21.353333333333335</v>
       </c>
     </row>
@@ -1889,10 +1899,10 @@
       <c r="A13" s="1">
         <v>42339</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="2">
         <v>21</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="2">
         <v>21.048333333333332</v>
       </c>
     </row>
@@ -1900,10 +1910,10 @@
       <c r="A14" s="1">
         <v>42370</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="2">
         <v>21</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="2">
         <v>20.773</v>
       </c>
     </row>
@@ -1911,10 +1921,10 @@
       <c r="A15" s="1">
         <v>42401</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="2">
         <v>22</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="2">
         <v>20.546000000000003</v>
       </c>
     </row>
@@ -1922,10 +1932,10 @@
       <c r="A16" s="1">
         <v>42430</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="2">
         <v>22</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="2">
         <v>20.388999999999999</v>
       </c>
     </row>
@@ -1933,10 +1943,10 @@
       <c r="A17" s="1">
         <v>42461</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="2">
         <v>23</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="2">
         <v>20.296333333333333</v>
       </c>
     </row>
@@ -1944,10 +1954,10 @@
       <c r="A18" s="1">
         <v>42491</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="2">
         <v>23.333333333333332</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="2">
         <v>20.227666666666664</v>
       </c>
     </row>
@@ -1955,10 +1965,10 @@
       <c r="A19" s="1">
         <v>42522</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" s="2">
         <v>24</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="2">
         <v>20.134666666666664</v>
       </c>
     </row>
@@ -1966,10 +1976,10 @@
       <c r="A20" s="1">
         <v>42552</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20" s="2">
         <v>24.333333333333332</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="2">
         <v>19.980333333333331</v>
       </c>
     </row>
@@ -1977,10 +1987,10 @@
       <c r="A21" s="1">
         <v>42583</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" s="2">
         <v>26.666666666666668</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="2">
         <v>19.748333333333331</v>
       </c>
     </row>
@@ -1988,10 +1998,10 @@
       <c r="A22" s="1">
         <v>42614</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="2">
         <v>26.666666666666668</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="2">
         <v>19.462</v>
       </c>
     </row>
@@ -1999,10 +2009,10 @@
       <c r="A23" s="1">
         <v>42644</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" s="2">
         <v>25.333333333333332</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23" s="2">
         <v>19.156333333333333</v>
       </c>
     </row>
@@ -2010,10 +2020,10 @@
       <c r="A24" s="1">
         <v>42675</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="2">
         <v>23.333333333333332</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C24" s="2">
         <v>18.839666666666663</v>
       </c>
     </row>
@@ -2021,10 +2031,10 @@
       <c r="A25" s="1">
         <v>42705</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B25" s="2">
         <v>23.333333333333332</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C25" s="2">
         <v>18.495666666666665</v>
       </c>
     </row>
@@ -2032,10 +2042,10 @@
       <c r="A26" s="1">
         <v>42736</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26" s="2">
         <v>24.666666666666668</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C26" s="2">
         <v>18.227</v>
       </c>
     </row>
@@ -2043,10 +2053,10 @@
       <c r="A27" s="1">
         <v>42767</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B27" s="2">
         <v>24.333333333333332</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C27" s="2">
         <v>17.995333333333335</v>
       </c>
     </row>
@@ -2054,10 +2064,10 @@
       <c r="A28" s="1">
         <v>42795</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B28" s="2">
         <v>24.333333333333332</v>
       </c>
-      <c r="C28" s="3">
+      <c r="C28" s="2">
         <v>17.801999999999996</v>
       </c>
     </row>
@@ -2065,10 +2075,10 @@
       <c r="A29" s="1">
         <v>42826</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B29" s="2">
         <v>25</v>
       </c>
-      <c r="C29" s="3">
+      <c r="C29" s="2">
         <v>17.507999999999999</v>
       </c>
     </row>
@@ -2076,10 +2086,10 @@
       <c r="A30" s="1">
         <v>42856</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B30" s="2">
         <v>25</v>
       </c>
-      <c r="C30" s="3">
+      <c r="C30" s="2">
         <v>17.093</v>
       </c>
     </row>
@@ -2087,10 +2097,10 @@
       <c r="A31" s="1">
         <v>42887</v>
       </c>
-      <c r="B31" s="3">
+      <c r="B31" s="2">
         <v>26.333333333333332</v>
       </c>
-      <c r="C31" s="3">
+      <c r="C31" s="2">
         <v>16.494333333333334</v>
       </c>
     </row>
@@ -2098,10 +2108,10 @@
       <c r="A32" s="1">
         <v>42917</v>
       </c>
-      <c r="B32" s="3">
+      <c r="B32" s="2">
         <v>26.666666666666668</v>
       </c>
-      <c r="C32" s="3">
+      <c r="C32" s="2">
         <v>15.71</v>
       </c>
     </row>
@@ -2109,10 +2119,10 @@
       <c r="A33" s="1">
         <v>42948</v>
       </c>
-      <c r="B33" s="3">
+      <c r="B33" s="2">
         <v>27.666666666666668</v>
       </c>
-      <c r="C33" s="3">
+      <c r="C33" s="2">
         <v>14.818666666666665</v>
       </c>
     </row>
@@ -2120,10 +2130,10 @@
       <c r="A34" s="1">
         <v>42979</v>
       </c>
-      <c r="B34" s="3">
+      <c r="B34" s="2">
         <v>27.333333333333332</v>
       </c>
-      <c r="C34" s="3">
+      <c r="C34" s="2">
         <v>13.959333333333333</v>
       </c>
     </row>
@@ -2131,10 +2141,10 @@
       <c r="A35" s="1">
         <v>43009</v>
       </c>
-      <c r="B35" s="3">
+      <c r="B35" s="2">
         <v>27.666666666666668</v>
       </c>
-      <c r="C35" s="3">
+      <c r="C35" s="2">
         <v>13.296333333333331</v>
       </c>
     </row>
@@ -2142,10 +2152,10 @@
       <c r="A36" s="1">
         <v>43040</v>
       </c>
-      <c r="B36" s="3">
+      <c r="B36" s="2">
         <v>28</v>
       </c>
-      <c r="C36" s="3">
+      <c r="C36" s="2">
         <v>12.982333333333331</v>
       </c>
     </row>
@@ -2153,10 +2163,10 @@
       <c r="A37" s="1">
         <v>43070</v>
       </c>
-      <c r="B37" s="3">
+      <c r="B37" s="2">
         <v>28.333333333333332</v>
       </c>
-      <c r="C37" s="3">
+      <c r="C37" s="2">
         <v>13.077666666666667</v>
       </c>
     </row>
@@ -2164,10 +2174,10 @@
       <c r="A38" s="1">
         <v>43101</v>
       </c>
-      <c r="B38" s="3">
+      <c r="B38" s="2">
         <v>27.666666666666668</v>
       </c>
-      <c r="C38" s="3">
+      <c r="C38" s="2">
         <v>13.539333333333333</v>
       </c>
     </row>
@@ -2175,10 +2185,10 @@
       <c r="A39" s="1">
         <v>43132</v>
       </c>
-      <c r="B39" s="3">
+      <c r="B39" s="2">
         <v>27</v>
       </c>
-      <c r="C39" s="3">
+      <c r="C39" s="2">
         <v>14.114666666666666</v>
       </c>
     </row>
@@ -2186,10 +2196,10 @@
       <c r="A40" s="1">
         <v>43160</v>
       </c>
-      <c r="B40" s="3">
+      <c r="B40" s="2">
         <v>27</v>
       </c>
-      <c r="C40" s="3">
+      <c r="C40" s="2">
         <v>14.677000000000001</v>
       </c>
     </row>
@@ -2197,10 +2207,10 @@
       <c r="A41" s="1">
         <v>43191</v>
       </c>
-      <c r="B41" s="3">
+      <c r="B41" s="2">
         <v>27.333333333333332</v>
       </c>
-      <c r="C41" s="3">
+      <c r="C41" s="2">
         <v>15.122666666666667</v>
       </c>
     </row>
@@ -2208,10 +2218,10 @@
       <c r="A42" s="1">
         <v>43221</v>
       </c>
-      <c r="B42" s="3">
+      <c r="B42" s="2">
         <v>28</v>
       </c>
-      <c r="C42" s="3">
+      <c r="C42" s="2">
         <v>15.543666666666667</v>
       </c>
     </row>
@@ -2219,10 +2229,10 @@
       <c r="A43" s="1">
         <v>43252</v>
       </c>
-      <c r="B43" s="3">
+      <c r="B43" s="2">
         <v>28</v>
       </c>
-      <c r="C43" s="3">
+      <c r="C43" s="2">
         <v>15.949</v>
       </c>
     </row>
@@ -2230,10 +2240,10 @@
       <c r="A44" s="1">
         <v>43282</v>
       </c>
-      <c r="B44" s="3">
+      <c r="B44" s="2">
         <v>27.333333333333332</v>
       </c>
-      <c r="C44" s="3">
+      <c r="C44" s="2">
         <v>16.357333333333333</v>
       </c>
     </row>
@@ -2241,10 +2251,10 @@
       <c r="A45" s="1">
         <v>43313</v>
       </c>
-      <c r="B45" s="3">
+      <c r="B45" s="2">
         <v>27.666666666666668</v>
       </c>
-      <c r="C45" s="3">
+      <c r="C45" s="2">
         <v>16.785333333333334</v>
       </c>
     </row>
@@ -2252,10 +2262,10 @@
       <c r="A46" s="1">
         <v>43344</v>
       </c>
-      <c r="B46" s="3">
+      <c r="B46" s="2">
         <v>28.333333333333332</v>
       </c>
-      <c r="C46" s="3">
+      <c r="C46" s="2">
         <v>17.238333333333333</v>
       </c>
     </row>
@@ -2263,10 +2273,10 @@
       <c r="A47" s="1">
         <v>43374</v>
       </c>
-      <c r="B47" s="3">
+      <c r="B47" s="2">
         <v>29.666666666666668</v>
       </c>
-      <c r="C47" s="3">
+      <c r="C47" s="2">
         <v>17.714333333333332</v>
       </c>
     </row>
@@ -2274,10 +2284,10 @@
       <c r="A48" s="1">
         <v>43405</v>
       </c>
-      <c r="B48" s="3">
+      <c r="B48" s="2">
         <v>30.333333333333332</v>
       </c>
-      <c r="C48" s="3">
+      <c r="C48" s="2">
         <v>18.178999999999998</v>
       </c>
     </row>
@@ -2285,10 +2295,10 @@
       <c r="A49" s="1">
         <v>43435</v>
       </c>
-      <c r="B49" s="3">
+      <c r="B49" s="2">
         <v>31</v>
       </c>
-      <c r="C49" s="3">
+      <c r="C49" s="2">
         <v>18.574000000000002</v>
       </c>
     </row>
@@ -2296,10 +2306,10 @@
       <c r="A50" s="1">
         <v>43466</v>
       </c>
-      <c r="B50" s="3">
+      <c r="B50" s="2">
         <v>37.333333333333336</v>
       </c>
-      <c r="C50" s="3">
+      <c r="C50" s="2">
         <v>18.816333333333333</v>
       </c>
     </row>
@@ -2307,10 +2317,10 @@
       <c r="A51" s="1">
         <v>43497</v>
       </c>
-      <c r="B51" s="3">
+      <c r="B51" s="2">
         <v>37.333333333333336</v>
       </c>
-      <c r="C51" s="3">
+      <c r="C51" s="2">
         <v>18.864999999999998</v>
       </c>
     </row>
@@ -2318,10 +2328,10 @@
       <c r="A52" s="1">
         <v>43525</v>
       </c>
-      <c r="B52" s="3">
+      <c r="B52" s="2">
         <v>36.666666666666664</v>
       </c>
-      <c r="C52" s="3">
+      <c r="C52" s="2">
         <v>18.714333333333332</v>
       </c>
     </row>
@@ -2329,10 +2339,10 @@
       <c r="A53" s="1">
         <v>43556</v>
       </c>
-      <c r="B53" s="3">
+      <c r="B53" s="2">
         <v>28.666666666666668</v>
       </c>
-      <c r="C53" s="3">
+      <c r="C53" s="2">
         <v>18.423333333333332</v>
       </c>
     </row>
@@ -2340,10 +2350,10 @@
       <c r="A54" s="1">
         <v>43586</v>
       </c>
-      <c r="B54" s="3">
+      <c r="B54" s="2">
         <v>28.666666666666668</v>
       </c>
-      <c r="C54" s="3">
+      <c r="C54" s="2">
         <v>18.046999999999997</v>
       </c>
     </row>
@@ -2351,10 +2361,10 @@
       <c r="A55" s="1">
         <v>43617</v>
       </c>
-      <c r="B55" s="3">
+      <c r="B55" s="2">
         <v>28.666666666666668</v>
       </c>
-      <c r="C55" s="3">
+      <c r="C55" s="2">
         <v>17.650000000000002</v>
       </c>
     </row>
@@ -2362,10 +2372,10 @@
       <c r="A56" s="1">
         <v>43647</v>
       </c>
-      <c r="B56" s="3">
+      <c r="B56" s="2">
         <v>30.666666666666668</v>
       </c>
-      <c r="C56" s="3">
+      <c r="C56" s="2">
         <v>17.286000000000001</v>
       </c>
     </row>
@@ -2373,10 +2383,10 @@
       <c r="A57" s="1">
         <v>43678</v>
       </c>
-      <c r="B57" s="3">
+      <c r="B57" s="2">
         <v>30.333333333333332</v>
       </c>
-      <c r="C57" s="3">
+      <c r="C57" s="2">
         <v>16.980999999999998</v>
       </c>
     </row>
@@ -2384,10 +2394,10 @@
       <c r="A58" s="1">
         <v>43709</v>
       </c>
-      <c r="B58" s="3">
+      <c r="B58" s="2">
         <v>31</v>
       </c>
-      <c r="C58" s="3">
+      <c r="C58" s="2">
         <v>16.719666666666665</v>
       </c>
     </row>
@@ -2395,10 +2405,10 @@
       <c r="A59" s="1">
         <v>43739</v>
       </c>
-      <c r="B59" s="3">
+      <c r="B59" s="2">
         <v>31</v>
       </c>
-      <c r="C59" s="3">
+      <c r="C59" s="2">
         <v>16.471666666666668</v>
       </c>
     </row>
@@ -2406,10 +2416,10 @@
       <c r="A60" s="1">
         <v>43770</v>
       </c>
-      <c r="B60" s="3">
+      <c r="B60" s="2">
         <v>30.333333333333332</v>
       </c>
-      <c r="C60" s="3">
+      <c r="C60" s="2">
         <v>16.199666666666669</v>
       </c>
     </row>
@@ -2417,10 +2427,10 @@
       <c r="A61" s="1">
         <v>43800</v>
       </c>
-      <c r="B61" s="3">
+      <c r="B61" s="2">
         <v>28.333333333333332</v>
       </c>
-      <c r="C61" s="3">
+      <c r="C61" s="2">
         <v>15.900333333333331</v>
       </c>
     </row>
@@ -2428,10 +2438,10 @@
       <c r="A62" s="1">
         <v>43831</v>
       </c>
-      <c r="B62" s="3">
+      <c r="B62" s="2">
         <v>30.666666666666668</v>
       </c>
-      <c r="C62" s="3">
+      <c r="C62" s="2">
         <v>15.583999999999998</v>
       </c>
     </row>
@@ -2439,10 +2449,10 @@
       <c r="A63" s="1">
         <v>43862</v>
       </c>
-      <c r="B63" s="3">
+      <c r="B63" s="2">
         <v>30</v>
       </c>
-      <c r="C63" s="3">
+      <c r="C63" s="2">
         <v>15.287000000000001</v>
       </c>
     </row>
@@ -2450,10 +2460,10 @@
       <c r="A64" s="1">
         <v>43891</v>
       </c>
-      <c r="B64" s="3">
+      <c r="B64" s="2">
         <v>29</v>
       </c>
-      <c r="C64" s="3">
+      <c r="C64" s="2">
         <v>15.027666666666667</v>
       </c>
     </row>
@@ -2461,10 +2471,10 @@
       <c r="A65" s="1">
         <v>43922</v>
       </c>
-      <c r="B65" s="3">
+      <c r="B65" s="2">
         <v>21.666666666666668</v>
       </c>
-      <c r="C65" s="3">
+      <c r="C65" s="2">
         <v>58.724333333333334</v>
       </c>
     </row>
@@ -2472,10 +2482,10 @@
       <c r="A66" s="1">
         <v>43952</v>
       </c>
-      <c r="B66" s="3">
+      <c r="B66" s="2">
         <v>21.666666666666668</v>
       </c>
-      <c r="C66" s="3">
+      <c r="C66" s="2">
         <v>99.879666666666665</v>
       </c>
     </row>
@@ -2483,10 +2493,10 @@
       <c r="A67" s="1">
         <v>43983</v>
       </c>
-      <c r="B67" s="3">
+      <c r="B67" s="2">
         <v>21</v>
       </c>
-      <c r="C67" s="3">
+      <c r="C67" s="2">
         <v>133.51733333333334</v>
       </c>
     </row>
@@ -2494,10 +2504,10 @@
       <c r="A68" s="1">
         <v>44013</v>
       </c>
-      <c r="B68" s="3">
+      <c r="B68" s="2">
         <v>23</v>
       </c>
-      <c r="C68" s="3">
+      <c r="C68" s="2">
         <v>119.90599999999999</v>
       </c>
     </row>
@@ -2505,10 +2515,10 @@
       <c r="A69" s="1">
         <v>44044</v>
       </c>
-      <c r="B69" s="3">
+      <c r="B69" s="2">
         <v>21</v>
       </c>
-      <c r="C69" s="3">
+      <c r="C69" s="2">
         <v>103.06866666666667</v>
       </c>
     </row>
@@ -2516,10 +2526,10 @@
       <c r="A70" s="1">
         <v>44075</v>
       </c>
-      <c r="B70" s="3">
+      <c r="B70" s="2">
         <v>20</v>
       </c>
-      <c r="C70" s="3">
+      <c r="C70" s="2">
         <v>92.309666666666658</v>
       </c>
     </row>
@@ -2527,10 +2537,10 @@
       <c r="A71" s="1">
         <v>44105</v>
       </c>
-      <c r="B71" s="3">
+      <c r="B71" s="2">
         <v>23.333333333333332</v>
       </c>
-      <c r="C71" s="3">
+      <c r="C71" s="2">
         <v>81.519666666666666</v>
       </c>
     </row>
@@ -2538,10 +2548,10 @@
       <c r="A72" s="1">
         <v>44136</v>
       </c>
-      <c r="B72" s="3">
+      <c r="B72" s="2">
         <v>27.333333333333332</v>
       </c>
-      <c r="C72" s="3">
+      <c r="C72" s="2">
         <v>75.272333333333336</v>
       </c>
     </row>
@@ -2549,10 +2559,10 @@
       <c r="A73" s="1">
         <v>44166</v>
       </c>
-      <c r="B73" s="3">
+      <c r="B73" s="2">
         <v>31</v>
       </c>
-      <c r="C73" s="3">
+      <c r="C73" s="2">
         <v>70.195333333333338</v>
       </c>
     </row>
@@ -2560,10 +2570,10 @@
       <c r="A74" s="1">
         <v>44197</v>
       </c>
-      <c r="B74" s="3">
+      <c r="B74" s="2">
         <v>29.333333333333332</v>
       </c>
-      <c r="C74" s="3">
+      <c r="C74" s="2">
         <v>67.042999999999992</v>
       </c>
     </row>
@@ -2571,10 +2581,10 @@
       <c r="A75" s="1">
         <v>44228</v>
       </c>
-      <c r="B75" s="3">
+      <c r="B75" s="2">
         <v>27.333333333333332</v>
       </c>
-      <c r="C75" s="3">
+      <c r="C75" s="2">
         <v>64.557666666666663</v>
       </c>
     </row>
@@ -2582,10 +2592,10 @@
       <c r="A76" s="1">
         <v>44256</v>
       </c>
-      <c r="B76" s="3">
+      <c r="B76" s="2">
         <v>28</v>
       </c>
-      <c r="C76" s="3">
+      <c r="C76" s="2">
         <v>60.796333333333337</v>
       </c>
     </row>
@@ -2593,10 +2603,10 @@
       <c r="A77" s="1">
         <v>44287</v>
       </c>
-      <c r="B77" s="3">
+      <c r="B77" s="2">
         <v>33.666666666666664</v>
       </c>
-      <c r="C77" s="3">
+      <c r="C77" s="2">
         <v>57.010666666666673</v>
       </c>
     </row>
@@ -2604,10 +2614,10 @@
       <c r="A78" s="1">
         <v>44317</v>
       </c>
-      <c r="B78" s="3">
+      <c r="B78" s="2">
         <v>39</v>
       </c>
-      <c r="C78" s="3">
+      <c r="C78" s="2">
         <v>51.80866666666666</v>
       </c>
     </row>
@@ -2615,10 +2625,10 @@
       <c r="A79" s="1">
         <v>44348</v>
       </c>
-      <c r="B79" s="3">
+      <c r="B79" s="2">
         <v>43</v>
       </c>
-      <c r="C79" s="3">
+      <c r="C79" s="2">
         <v>46.959333333333326</v>
       </c>
     </row>
@@ -2626,10 +2636,10 @@
       <c r="A80" s="1">
         <v>44378</v>
       </c>
-      <c r="B80" s="3">
+      <c r="B80" s="2">
         <v>45.666666666666664</v>
       </c>
-      <c r="C80" s="3">
+      <c r="C80" s="2">
         <v>41.664000000000001</v>
       </c>
     </row>
@@ -2637,10 +2647,10 @@
       <c r="A81" s="1">
         <v>44409</v>
       </c>
-      <c r="B81" s="3">
+      <c r="B81" s="2">
         <v>44.666666666666664</v>
       </c>
-      <c r="C81" s="3">
+      <c r="C81" s="2">
         <v>36.777999999999999</v>
       </c>
     </row>
@@ -2648,10 +2658,10 @@
       <c r="A82" s="1">
         <v>44440</v>
       </c>
-      <c r="B82" s="3">
+      <c r="B82" s="2">
         <v>43</v>
       </c>
-      <c r="C82" s="3">
+      <c r="C82" s="2">
         <v>31.407</v>
       </c>
     </row>
@@ -2659,10 +2669,10 @@
       <c r="A83" s="1">
         <v>44470</v>
       </c>
-      <c r="B83" s="3">
+      <c r="B83" s="2">
         <v>39.333333333333336</v>
       </c>
-      <c r="C83" s="3">
+      <c r="C83" s="2">
         <v>26.51</v>
       </c>
     </row>
@@ -2670,10 +2680,10 @@
       <c r="A84" s="1">
         <v>44501</v>
       </c>
-      <c r="B84" s="3">
+      <c r="B84" s="2">
         <v>39</v>
       </c>
-      <c r="C84" s="3">
+      <c r="C84" s="2">
         <v>23.046000000000003</v>
       </c>
     </row>
@@ -2681,10 +2691,10 @@
       <c r="A85" s="1">
         <v>44531</v>
       </c>
-      <c r="B85" s="3">
+      <c r="B85" s="2">
         <v>39.333333333333336</v>
       </c>
-      <c r="C85" s="3">
+      <c r="C85" s="2">
         <v>21.242333333333335</v>
       </c>
     </row>
@@ -2692,10 +2702,10 @@
       <c r="A86" s="1">
         <v>44562</v>
       </c>
-      <c r="B86" s="3">
+      <c r="B86" s="2">
         <v>40</v>
       </c>
-      <c r="C86" s="3">
+      <c r="C86" s="2">
         <v>20.978666666666665</v>
       </c>
     </row>
@@ -2703,10 +2713,10 @@
       <c r="A87" s="1">
         <v>44593</v>
       </c>
-      <c r="B87" s="3">
+      <c r="B87" s="2">
         <v>41.333333333333336</v>
       </c>
-      <c r="C87" s="3">
+      <c r="C87" s="2">
         <v>21.002666666666666</v>
       </c>
     </row>
@@ -2714,10 +2724,10 @@
       <c r="A88" s="1">
         <v>44621</v>
       </c>
-      <c r="B88" s="3">
+      <c r="B88" s="2">
         <v>42</v>
       </c>
-      <c r="C88" s="3">
+      <c r="C88" s="2">
         <v>21.224333333333334</v>
       </c>
     </row>
@@ -2725,10 +2735,10 @@
       <c r="A89" s="1">
         <v>44652</v>
       </c>
-      <c r="B89" s="3">
+      <c r="B89" s="2">
         <v>41</v>
       </c>
-      <c r="C89" s="3">
+      <c r="C89" s="2">
         <v>21.520333333333337</v>
       </c>
     </row>
@@ -2736,10 +2746,10 @@
       <c r="A90" s="1">
         <v>44682</v>
       </c>
-      <c r="B90" s="3">
+      <c r="B90" s="2">
         <v>40.333333333333336</v>
       </c>
-      <c r="C90" s="3">
+      <c r="C90" s="2">
         <v>21.824666666666669</v>
       </c>
     </row>
@@ -2747,10 +2757,10 @@
       <c r="A91" s="1">
         <v>44713</v>
       </c>
-      <c r="B91" s="3">
+      <c r="B91" s="2">
         <v>39</v>
       </c>
-      <c r="C91" s="3">
+      <c r="C91" s="2">
         <v>22.072333333333333</v>
       </c>
     </row>
@@ -2758,10 +2768,10 @@
       <c r="A92" s="1">
         <v>44743</v>
       </c>
-      <c r="B92" s="3">
+      <c r="B92" s="2">
         <v>42.333333333333336</v>
       </c>
-      <c r="C92" s="3">
+      <c r="C92" s="2">
         <v>22.248333333333335</v>
       </c>
     </row>
@@ -2769,10 +2779,10 @@
       <c r="A93" s="1">
         <v>44774</v>
       </c>
-      <c r="B93" s="3">
+      <c r="B93" s="2">
         <v>42</v>
       </c>
-      <c r="C93" s="3">
+      <c r="C93" s="2">
         <v>22.383666666666667</v>
       </c>
     </row>
@@ -2780,10 +2790,10 @@
       <c r="A94" s="1">
         <v>44805</v>
       </c>
-      <c r="B94" s="3">
+      <c r="B94" s="2">
         <v>42</v>
       </c>
-      <c r="C94" s="3">
+      <c r="C94" s="2">
         <v>22.459999999999997</v>
       </c>
     </row>
@@ -2791,10 +2801,10 @@
       <c r="A95" s="1">
         <v>44835</v>
       </c>
-      <c r="B95" s="3">
+      <c r="B95" s="2">
         <v>37.333333333333336</v>
       </c>
-      <c r="C95" s="3">
+      <c r="C95" s="2">
         <v>22.460333333333335</v>
       </c>
     </row>
@@ -2802,10 +2812,10 @@
       <c r="A96" s="1">
         <v>44866</v>
       </c>
-      <c r="B96" s="3">
+      <c r="B96" s="2">
         <v>35.666666666666664</v>
       </c>
-      <c r="C96" s="3">
+      <c r="C96" s="2">
         <v>22.345333333333333</v>
       </c>
     </row>
@@ -2813,10 +2823,10 @@
       <c r="A97" s="1">
         <v>44896</v>
       </c>
-      <c r="B97" s="3">
+      <c r="B97" s="2">
         <v>35.666666666666664</v>
       </c>
-      <c r="C97" s="3">
+      <c r="C97" s="2">
         <v>22.104666666666663</v>
       </c>
     </row>
@@ -2824,10 +2834,10 @@
       <c r="A98" s="1">
         <v>44927</v>
       </c>
-      <c r="B98" s="3">
+      <c r="B98" s="2">
         <v>36</v>
       </c>
-      <c r="C98" s="3">
+      <c r="C98" s="2">
         <v>21.719666666666665</v>
       </c>
     </row>
@@ -2835,10 +2845,10 @@
       <c r="A99" s="1">
         <v>44958</v>
       </c>
-      <c r="B99" s="3">
+      <c r="B99" s="2">
         <v>36.333333333333336</v>
       </c>
-      <c r="C99" s="3">
+      <c r="C99" s="2">
         <v>21.198333333333334</v>
       </c>
     </row>
@@ -2846,10 +2856,10 @@
       <c r="A100" s="1">
         <v>44986</v>
       </c>
-      <c r="B100" s="3">
+      <c r="B100" s="2">
         <v>35</v>
       </c>
-      <c r="C100" s="3">
+      <c r="C100" s="2">
         <v>20.578333333333333</v>
       </c>
     </row>
@@ -2857,10 +2867,10 @@
       <c r="A101" s="1">
         <v>45017</v>
       </c>
-      <c r="B101" s="3">
+      <c r="B101" s="2">
         <v>35.333333333333336</v>
       </c>
-      <c r="C101" s="3">
+      <c r="C101" s="2">
         <v>19.939666666666668</v>
       </c>
     </row>
@@ -2868,10 +2878,10 @@
       <c r="A102" s="1">
         <v>45047</v>
       </c>
-      <c r="B102" s="3">
+      <c r="B102" s="2">
         <v>34.666666666666664</v>
       </c>
-      <c r="C102" s="3">
+      <c r="C102" s="2">
         <v>19.408666666666665</v>
       </c>
     </row>
@@ -2879,10 +2889,10 @@
       <c r="A103" s="1">
         <v>45078</v>
       </c>
-      <c r="B103" s="3">
+      <c r="B103" s="2">
         <v>34</v>
       </c>
-      <c r="C103" s="3">
+      <c r="C103" s="2">
         <v>19.088666666666668</v>
       </c>
     </row>
@@ -2890,10 +2900,10 @@
       <c r="A104" s="1">
         <v>45108</v>
       </c>
-      <c r="B104" s="3">
+      <c r="B104" s="2">
         <v>32.333333333333336</v>
       </c>
-      <c r="C104" s="3">
+      <c r="C104" s="2">
         <v>19.037000000000003</v>
       </c>
     </row>
@@ -2901,10 +2911,10 @@
       <c r="A105" s="1">
         <v>45139</v>
       </c>
-      <c r="B105" s="3">
+      <c r="B105" s="2">
         <v>33</v>
       </c>
-      <c r="C105" s="3">
+      <c r="C105" s="2">
         <v>19.24366666666667</v>
       </c>
     </row>
@@ -2912,10 +2922,10 @@
       <c r="A106" s="1">
         <v>45170</v>
       </c>
-      <c r="B106" s="3">
+      <c r="B106" s="2">
         <v>33.333333333333336</v>
       </c>
-      <c r="C106" s="3">
+      <c r="C106" s="2">
         <v>19.643000000000001</v>
       </c>
     </row>
@@ -2923,10 +2933,10 @@
       <c r="A107" s="1">
         <v>45200</v>
       </c>
-      <c r="B107" s="3">
+      <c r="B107" s="2">
         <v>32.333333333333336</v>
       </c>
-      <c r="C107" s="3">
+      <c r="C107" s="2">
         <v>20.097666666666665</v>
       </c>
     </row>
@@ -2934,10 +2944,10 @@
       <c r="A108" s="1">
         <v>45231</v>
       </c>
-      <c r="B108" s="3">
+      <c r="B108" s="2">
         <v>30.333333333333332</v>
       </c>
-      <c r="C108" s="3">
+      <c r="C108" s="2">
         <v>20.418333333333333</v>
       </c>
     </row>
@@ -2945,10 +2955,10 @@
       <c r="A109" s="1">
         <v>45261</v>
       </c>
-      <c r="B109" s="3">
+      <c r="B109" s="2">
         <v>29</v>
       </c>
-      <c r="C109" s="3">
+      <c r="C109" s="2">
         <v>20.550333333333331</v>
       </c>
     </row>
@@ -2956,10 +2966,10 @@
       <c r="A110" s="1">
         <v>45292</v>
       </c>
-      <c r="B110" s="3">
+      <c r="B110" s="2">
         <v>27.333333333333332</v>
       </c>
-      <c r="C110" s="3">
+      <c r="C110" s="2">
         <v>20.663666666666668</v>
       </c>
     </row>
@@ -2967,10 +2977,10 @@
       <c r="A111" s="1">
         <v>45323</v>
       </c>
-      <c r="B111" s="3">
+      <c r="B111" s="2">
         <v>28</v>
       </c>
-      <c r="C111" s="3">
+      <c r="C111" s="2">
         <v>20.832666666666665</v>
       </c>
     </row>
@@ -2983,1449 +2993,1449 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7A5DA13-9001-BE44-B4A7-5F44FEC0D447}">
   <dimension ref="A1:F72"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="A1:F72"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="5">
+      <c r="A2" s="4">
         <v>43101</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="5">
         <v>6</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="5">
         <v>44.1</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="5">
         <v>31</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="5">
         <v>10.199999999999999</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="5">
         <v>8.8000000000000007</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="5">
+      <c r="A3" s="4">
         <v>43132</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="5">
         <v>6</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="5">
         <v>44</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <v>31.2</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="5">
         <v>10.1</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="5">
         <v>8.8000000000000007</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="5">
+      <c r="A4" s="4">
         <v>43160</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="5">
         <v>5.9</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <v>43.8</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>31.6</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
         <v>10</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="5">
         <v>8.6999999999999993</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="5">
+      <c r="A5" s="4">
         <v>43191</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <v>5.8</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>43.5</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <v>31.9</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>10.1</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="5">
         <v>8.6999999999999993</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="5">
+      <c r="A6" s="4">
         <v>43221</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="5">
         <v>5.8</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <v>43.2</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>32.299999999999997</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <v>10.1</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="5">
         <v>8.6</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="5">
+      <c r="A7" s="4">
         <v>43252</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="5">
         <v>5.7</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <v>43</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <v>32.700000000000003</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="5">
         <v>10.1</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="5">
         <v>8.5</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="5">
+      <c r="A8" s="4">
         <v>43282</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="5">
         <v>5.6</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="5">
         <v>42.7</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="5">
         <v>33.1</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="5">
         <v>10.199999999999999</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="5">
         <v>8.4</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="5">
+      <c r="A9" s="4">
         <v>43313</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="5">
         <v>5.5</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <v>42.4</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="5">
         <v>33.5</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="5">
         <v>10.3</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="5">
         <v>8.3000000000000007</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="5">
+      <c r="A10" s="4">
         <v>43344</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="5">
         <v>5.5</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="5">
         <v>42.4</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="5">
         <v>33.700000000000003</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="5">
         <v>10.3</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="5">
         <v>8.1</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="5">
+      <c r="A11" s="4">
         <v>43374</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="5">
         <v>5.4</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="5">
         <v>42.1</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="5">
         <v>33.9</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="5">
         <v>10.5</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="5">
         <v>8.1999999999999993</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="5">
+      <c r="A12" s="4">
         <v>43405</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="5">
         <v>5.3</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="5">
         <v>42</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="5">
         <v>34</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="5">
         <v>10.6</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="5">
         <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="5">
+      <c r="A13" s="4">
         <v>43435</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="5">
         <v>5.3</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="5">
         <v>42.1</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="5">
         <v>34</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="5">
         <v>10.8</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F13" s="5">
         <v>7.8</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="5">
+      <c r="A14" s="4">
         <v>43466</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="5">
         <v>5.2</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="5">
         <v>42.1</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="5">
         <v>34.200000000000003</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E14" s="5">
         <v>11</v>
       </c>
-      <c r="F14" s="6">
+      <c r="F14" s="5">
         <v>7.6</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="5">
+      <c r="A15" s="4">
         <v>43497</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="5">
         <v>5.0999999999999996</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="5">
         <v>42.1</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="5">
         <v>34.200000000000003</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="5">
         <v>11.1</v>
       </c>
-      <c r="F15" s="6">
+      <c r="F15" s="5">
         <v>7.5</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="5">
+      <c r="A16" s="4">
         <v>43525</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="5">
         <v>5</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="5">
         <v>41.9</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16" s="5">
         <v>34.299999999999997</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E16" s="5">
         <v>11.2</v>
       </c>
-      <c r="F16" s="6">
+      <c r="F16" s="5">
         <v>7.5</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="5">
+      <c r="A17" s="4">
         <v>43556</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="5">
         <v>5</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="5">
         <v>41.9</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D17" s="5">
         <v>34.4</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="5">
         <v>11.3</v>
       </c>
-      <c r="F17" s="6">
+      <c r="F17" s="5">
         <v>7.4</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="5">
+      <c r="A18" s="4">
         <v>43586</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="5">
         <v>4.9000000000000004</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C18" s="5">
         <v>42</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D18" s="5">
         <v>34.4</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E18" s="5">
         <v>11.3</v>
       </c>
-      <c r="F18" s="6">
+      <c r="F18" s="5">
         <v>7.3</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="5">
+      <c r="A19" s="4">
         <v>43617</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B19" s="5">
         <v>4.9000000000000004</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="5">
         <v>42.1</v>
       </c>
-      <c r="D19" s="6">
+      <c r="D19" s="5">
         <v>34.6</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E19" s="5">
         <v>11.2</v>
       </c>
-      <c r="F19" s="6">
+      <c r="F19" s="5">
         <v>7.2</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="5">
+      <c r="A20" s="4">
         <v>43647</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B20" s="5">
         <v>4.9000000000000004</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C20" s="5">
         <v>42.5</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D20" s="5">
         <v>34.4</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E20" s="5">
         <v>11.1</v>
       </c>
-      <c r="F20" s="6">
+      <c r="F20" s="5">
         <v>7.2</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="5">
+      <c r="A21" s="4">
         <v>43678</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="5">
         <v>4.8</v>
       </c>
-      <c r="C21" s="6">
+      <c r="C21" s="5">
         <v>42.9</v>
       </c>
-      <c r="D21" s="6">
+      <c r="D21" s="5">
         <v>34.4</v>
       </c>
-      <c r="E21" s="6">
+      <c r="E21" s="5">
         <v>10.8</v>
       </c>
-      <c r="F21" s="6">
+      <c r="F21" s="5">
         <v>7.1</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="5">
+      <c r="A22" s="4">
         <v>43709</v>
       </c>
-      <c r="B22" s="6">
+      <c r="B22" s="5">
         <v>4.8</v>
       </c>
-      <c r="C22" s="6">
+      <c r="C22" s="5">
         <v>43.3</v>
       </c>
-      <c r="D22" s="6">
+      <c r="D22" s="5">
         <v>34.200000000000003</v>
       </c>
-      <c r="E22" s="6">
+      <c r="E22" s="5">
         <v>10.7</v>
       </c>
-      <c r="F22" s="6">
+      <c r="F22" s="5">
         <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="5">
+      <c r="A23" s="4">
         <v>43739</v>
       </c>
-      <c r="B23" s="6">
+      <c r="B23" s="5">
         <v>5</v>
       </c>
-      <c r="C23" s="6">
+      <c r="C23" s="5">
         <v>43.9</v>
       </c>
-      <c r="D23" s="6">
+      <c r="D23" s="5">
         <v>33.799999999999997</v>
       </c>
-      <c r="E23" s="6">
+      <c r="E23" s="5">
         <v>10.4</v>
       </c>
-      <c r="F23" s="6">
+      <c r="F23" s="5">
         <v>6.9</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="5">
+      <c r="A24" s="4">
         <v>43770</v>
       </c>
-      <c r="B24" s="6">
+      <c r="B24" s="5">
         <v>5</v>
       </c>
-      <c r="C24" s="6">
+      <c r="C24" s="5">
         <v>44.7</v>
       </c>
-      <c r="D24" s="6">
+      <c r="D24" s="5">
         <v>33.9</v>
       </c>
-      <c r="E24" s="6">
+      <c r="E24" s="5">
         <v>9.9</v>
       </c>
-      <c r="F24" s="6">
+      <c r="F24" s="5">
         <v>6.6</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="5">
+      <c r="A25" s="4">
         <v>43800</v>
       </c>
-      <c r="B25" s="6">
+      <c r="B25" s="5">
         <v>5.0999999999999996</v>
       </c>
-      <c r="C25" s="6">
+      <c r="C25" s="5">
         <v>45.5</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D25" s="5">
         <v>33.6</v>
       </c>
-      <c r="E25" s="6">
+      <c r="E25" s="5">
         <v>9.5</v>
       </c>
-      <c r="F25" s="6">
+      <c r="F25" s="5">
         <v>6.3</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="5">
+      <c r="A26" s="4">
         <v>43831</v>
       </c>
-      <c r="B26" s="6">
+      <c r="B26" s="5">
         <v>5.0999999999999996</v>
       </c>
-      <c r="C26" s="6">
+      <c r="C26" s="5">
         <v>46.4</v>
       </c>
-      <c r="D26" s="6">
+      <c r="D26" s="5">
         <v>33.299999999999997</v>
       </c>
-      <c r="E26" s="6">
+      <c r="E26" s="5">
         <v>9.1</v>
       </c>
-      <c r="F26" s="6">
+      <c r="F26" s="5">
         <v>6.1</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="5">
+      <c r="A27" s="4">
         <v>43862</v>
       </c>
-      <c r="B27" s="6">
+      <c r="B27" s="5">
         <v>5.2</v>
       </c>
-      <c r="C27" s="6">
+      <c r="C27" s="5">
         <v>46.8</v>
       </c>
-      <c r="D27" s="6">
+      <c r="D27" s="5">
         <v>33.1</v>
       </c>
-      <c r="E27" s="6">
+      <c r="E27" s="5">
         <v>8.9</v>
       </c>
-      <c r="F27" s="6">
+      <c r="F27" s="5">
         <v>5.9</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="5">
+      <c r="A28" s="4">
         <v>43891</v>
       </c>
-      <c r="B28" s="6">
+      <c r="B28" s="5">
         <v>5.5</v>
       </c>
-      <c r="C28" s="6">
+      <c r="C28" s="5">
         <v>47.1</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D28" s="5">
         <v>32.799999999999997</v>
       </c>
-      <c r="E28" s="6">
+      <c r="E28" s="5">
         <v>8.6999999999999993</v>
       </c>
-      <c r="F28" s="6">
+      <c r="F28" s="5">
         <v>5.9</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="5">
+      <c r="A29" s="4">
         <v>43922</v>
       </c>
-      <c r="B29" s="6">
+      <c r="B29" s="5">
         <v>5.9</v>
       </c>
-      <c r="C29" s="6">
+      <c r="C29" s="5">
         <v>47.5</v>
       </c>
-      <c r="D29" s="6">
+      <c r="D29" s="5">
         <v>32.4</v>
       </c>
-      <c r="E29" s="6">
+      <c r="E29" s="5">
         <v>8.5</v>
       </c>
-      <c r="F29" s="6">
+      <c r="F29" s="5">
         <v>5.8</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="5">
+      <c r="A30" s="4">
         <v>43952</v>
       </c>
-      <c r="B30" s="6">
+      <c r="B30" s="5">
         <v>6.3</v>
       </c>
-      <c r="C30" s="6">
+      <c r="C30" s="5">
         <v>47.8</v>
       </c>
-      <c r="D30" s="6">
+      <c r="D30" s="5">
         <v>31.8</v>
       </c>
-      <c r="E30" s="6">
+      <c r="E30" s="5">
         <v>8.3000000000000007</v>
       </c>
-      <c r="F30" s="6">
+      <c r="F30" s="5">
         <v>5.8</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" s="5">
+      <c r="A31" s="4">
         <v>43983</v>
       </c>
-      <c r="B31" s="6">
+      <c r="B31" s="5">
         <v>6.8</v>
       </c>
-      <c r="C31" s="6">
+      <c r="C31" s="5">
         <v>48.1</v>
       </c>
-      <c r="D31" s="6">
+      <c r="D31" s="5">
         <v>31.2</v>
       </c>
-      <c r="E31" s="6">
+      <c r="E31" s="5">
         <v>8.1999999999999993</v>
       </c>
-      <c r="F31" s="6">
+      <c r="F31" s="5">
         <v>5.7</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="5">
+      <c r="A32" s="4">
         <v>44013</v>
       </c>
-      <c r="B32" s="6">
+      <c r="B32" s="5">
         <v>7.6</v>
       </c>
-      <c r="C32" s="6">
+      <c r="C32" s="5">
         <v>48.2</v>
       </c>
-      <c r="D32" s="6">
+      <c r="D32" s="5">
         <v>30.5</v>
       </c>
-      <c r="E32" s="6">
+      <c r="E32" s="5">
         <v>8.1</v>
       </c>
-      <c r="F32" s="6">
+      <c r="F32" s="5">
         <v>5.6</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="5">
+      <c r="A33" s="4">
         <v>44044</v>
       </c>
-      <c r="B33" s="6">
+      <c r="B33" s="5">
         <v>8.6999999999999993</v>
       </c>
-      <c r="C33" s="6">
+      <c r="C33" s="5">
         <v>47.8</v>
       </c>
-      <c r="D33" s="6">
+      <c r="D33" s="5">
         <v>29.8</v>
       </c>
-      <c r="E33" s="6">
+      <c r="E33" s="5">
         <v>8</v>
       </c>
-      <c r="F33" s="6">
+      <c r="F33" s="5">
         <v>5.6</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="5">
+      <c r="A34" s="4">
         <v>44075</v>
       </c>
-      <c r="B34" s="6">
+      <c r="B34" s="5">
         <v>10.1</v>
       </c>
-      <c r="C34" s="6">
+      <c r="C34" s="5">
         <v>47.4</v>
       </c>
-      <c r="D34" s="6">
+      <c r="D34" s="5">
         <v>29.4</v>
       </c>
-      <c r="E34" s="6">
+      <c r="E34" s="5">
         <v>7.9</v>
       </c>
-      <c r="F34" s="6">
+      <c r="F34" s="5">
         <v>5.2</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" s="5">
+      <c r="A35" s="4">
         <v>44105</v>
       </c>
-      <c r="B35" s="6">
+      <c r="B35" s="5">
         <v>11.9</v>
       </c>
-      <c r="C35" s="6">
+      <c r="C35" s="5">
         <v>46.5</v>
       </c>
-      <c r="D35" s="6">
+      <c r="D35" s="5">
         <v>28.6</v>
       </c>
-      <c r="E35" s="6">
+      <c r="E35" s="5">
         <v>7.8</v>
       </c>
-      <c r="F35" s="6">
+      <c r="F35" s="5">
         <v>5.2</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="5">
+      <c r="A36" s="4">
         <v>44136</v>
       </c>
-      <c r="B36" s="6">
+      <c r="B36" s="5">
         <v>13.5</v>
       </c>
-      <c r="C36" s="6">
+      <c r="C36" s="5">
         <v>45.7</v>
       </c>
-      <c r="D36" s="6">
+      <c r="D36" s="5">
         <v>27.9</v>
       </c>
-      <c r="E36" s="6">
+      <c r="E36" s="5">
         <v>7.7</v>
       </c>
-      <c r="F36" s="6">
+      <c r="F36" s="5">
         <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="5">
+      <c r="A37" s="4">
         <v>44166</v>
       </c>
-      <c r="B37" s="6">
+      <c r="B37" s="5">
         <v>15.5</v>
       </c>
-      <c r="C37" s="6">
+      <c r="C37" s="5">
         <v>44.7</v>
       </c>
-      <c r="D37" s="6">
+      <c r="D37" s="5">
         <v>27.1</v>
       </c>
-      <c r="E37" s="6">
+      <c r="E37" s="5">
         <v>7.7</v>
       </c>
-      <c r="F37" s="6">
+      <c r="F37" s="5">
         <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="5">
+      <c r="A38" s="4">
         <v>44197</v>
       </c>
-      <c r="B38" s="6">
+      <c r="B38" s="5">
         <v>17.2</v>
       </c>
-      <c r="C38" s="6">
+      <c r="C38" s="5">
         <v>43.8</v>
       </c>
-      <c r="D38" s="6">
+      <c r="D38" s="5">
         <v>26.4</v>
       </c>
-      <c r="E38" s="6">
+      <c r="E38" s="5">
         <v>7.6</v>
       </c>
-      <c r="F38" s="6">
+      <c r="F38" s="5">
         <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" s="5">
+      <c r="A39" s="4">
         <v>44228</v>
       </c>
-      <c r="B39" s="6">
+      <c r="B39" s="5">
         <v>19.2</v>
       </c>
-      <c r="C39" s="6">
+      <c r="C39" s="5">
         <v>42.8</v>
       </c>
-      <c r="D39" s="6">
+      <c r="D39" s="5">
         <v>25.6</v>
       </c>
-      <c r="E39" s="6">
+      <c r="E39" s="5">
         <v>7.4</v>
       </c>
-      <c r="F39" s="6">
+      <c r="F39" s="5">
         <v>5</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" s="5">
+      <c r="A40" s="4">
         <v>44256</v>
       </c>
-      <c r="B40" s="6">
+      <c r="B40" s="5">
         <v>21.4</v>
       </c>
-      <c r="C40" s="6">
+      <c r="C40" s="5">
         <v>41.7</v>
       </c>
-      <c r="D40" s="6">
+      <c r="D40" s="5">
         <v>24.7</v>
       </c>
-      <c r="E40" s="6">
+      <c r="E40" s="5">
         <v>7.3</v>
       </c>
-      <c r="F40" s="6">
+      <c r="F40" s="5">
         <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" s="5">
+      <c r="A41" s="4">
         <v>44287</v>
       </c>
-      <c r="B41" s="6">
+      <c r="B41" s="5">
         <v>22.8</v>
       </c>
-      <c r="C41" s="6">
+      <c r="C41" s="5">
         <v>41.1</v>
       </c>
-      <c r="D41" s="6">
+      <c r="D41" s="5">
         <v>24.2</v>
       </c>
-      <c r="E41" s="6">
+      <c r="E41" s="5">
         <v>7.1</v>
       </c>
-      <c r="F41" s="6">
+      <c r="F41" s="5">
         <v>4.8</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" s="5">
+      <c r="A42" s="4">
         <v>44317</v>
       </c>
-      <c r="B42" s="6">
+      <c r="B42" s="5">
         <v>24</v>
       </c>
-      <c r="C42" s="6">
+      <c r="C42" s="5">
         <v>40.799999999999997</v>
       </c>
-      <c r="D42" s="6">
+      <c r="D42" s="5">
         <v>23.5</v>
       </c>
-      <c r="E42" s="6">
+      <c r="E42" s="5">
         <v>7</v>
       </c>
-      <c r="F42" s="6">
+      <c r="F42" s="5">
         <v>4.8</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="5">
+      <c r="A43" s="4">
         <v>44348</v>
       </c>
-      <c r="B43" s="6">
+      <c r="B43" s="5">
         <v>25.3</v>
       </c>
-      <c r="C43" s="6">
+      <c r="C43" s="5">
         <v>40.5</v>
       </c>
-      <c r="D43" s="6">
+      <c r="D43" s="5">
         <v>22.7</v>
       </c>
-      <c r="E43" s="6">
+      <c r="E43" s="5">
         <v>6.8</v>
       </c>
-      <c r="F43" s="6">
+      <c r="F43" s="5">
         <v>4.7</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" s="5">
+      <c r="A44" s="4">
         <v>44378</v>
       </c>
-      <c r="B44" s="6">
+      <c r="B44" s="5">
         <v>26.3</v>
       </c>
-      <c r="C44" s="6">
+      <c r="C44" s="5">
         <v>40.200000000000003</v>
       </c>
-      <c r="D44" s="6">
+      <c r="D44" s="5">
         <v>22.2</v>
       </c>
-      <c r="E44" s="6">
+      <c r="E44" s="5">
         <v>6.7</v>
       </c>
-      <c r="F44" s="6">
+      <c r="F44" s="5">
         <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" s="5">
+      <c r="A45" s="4">
         <v>44409</v>
       </c>
-      <c r="B45" s="6">
+      <c r="B45" s="5">
         <v>27.5</v>
       </c>
-      <c r="C45" s="6">
+      <c r="C45" s="5">
         <v>39.799999999999997</v>
       </c>
-      <c r="D45" s="6">
+      <c r="D45" s="5">
         <v>21.6</v>
       </c>
-      <c r="E45" s="6">
+      <c r="E45" s="5">
         <v>6.5</v>
       </c>
-      <c r="F45" s="6">
+      <c r="F45" s="5">
         <v>4.5</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" s="5">
+      <c r="A46" s="4">
         <v>44440</v>
       </c>
-      <c r="B46" s="6">
+      <c r="B46" s="5">
         <v>28.7</v>
       </c>
-      <c r="C46" s="6">
+      <c r="C46" s="5">
         <v>39.4</v>
       </c>
-      <c r="D46" s="6">
+      <c r="D46" s="5">
         <v>21</v>
       </c>
-      <c r="E46" s="6">
+      <c r="E46" s="5">
         <v>6.4</v>
       </c>
-      <c r="F46" s="6">
+      <c r="F46" s="5">
         <v>4.5</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47" s="5">
+      <c r="A47" s="4">
         <v>44470</v>
       </c>
-      <c r="B47" s="6">
+      <c r="B47" s="5">
         <v>31.4</v>
       </c>
-      <c r="C47" s="6">
+      <c r="C47" s="5">
         <v>39.6</v>
       </c>
-      <c r="D47" s="6">
+      <c r="D47" s="5">
         <v>19.2</v>
       </c>
-      <c r="E47" s="6">
+      <c r="E47" s="5">
         <v>5.8</v>
       </c>
-      <c r="F47" s="6">
+      <c r="F47" s="5">
         <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48" s="5">
+      <c r="A48" s="4">
         <v>44501</v>
       </c>
-      <c r="B48" s="6">
+      <c r="B48" s="5">
         <v>32.4</v>
       </c>
-      <c r="C48" s="6">
+      <c r="C48" s="5">
         <v>39.299999999999997</v>
       </c>
-      <c r="D48" s="6">
+      <c r="D48" s="5">
         <v>18.7</v>
       </c>
-      <c r="E48" s="6">
+      <c r="E48" s="5">
         <v>5.7</v>
       </c>
-      <c r="F48" s="6">
+      <c r="F48" s="5">
         <v>3.9</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" s="5">
+      <c r="A49" s="4">
         <v>44531</v>
       </c>
-      <c r="B49" s="6">
+      <c r="B49" s="5">
         <v>33</v>
       </c>
-      <c r="C49" s="6">
+      <c r="C49" s="5">
         <v>39.200000000000003</v>
       </c>
-      <c r="D49" s="6">
+      <c r="D49" s="5">
         <v>18.3</v>
       </c>
-      <c r="E49" s="6">
+      <c r="E49" s="5">
         <v>5.6</v>
       </c>
-      <c r="F49" s="6">
+      <c r="F49" s="5">
         <v>3.9</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" s="5">
+      <c r="A50" s="4">
         <v>44562</v>
       </c>
-      <c r="B50" s="6">
+      <c r="B50" s="5">
         <v>33.6</v>
       </c>
-      <c r="C50" s="6">
+      <c r="C50" s="5">
         <v>39.200000000000003</v>
       </c>
-      <c r="D50" s="6">
+      <c r="D50" s="5">
         <v>17.899999999999999</v>
       </c>
-      <c r="E50" s="6">
+      <c r="E50" s="5">
         <v>5.5</v>
       </c>
-      <c r="F50" s="6">
+      <c r="F50" s="5">
         <v>3.8</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51" s="5">
+      <c r="A51" s="4">
         <v>44593</v>
       </c>
-      <c r="B51" s="6">
+      <c r="B51" s="5">
         <v>34.1</v>
       </c>
-      <c r="C51" s="6">
+      <c r="C51" s="5">
         <v>39.1</v>
       </c>
-      <c r="D51" s="6">
+      <c r="D51" s="5">
         <v>17.600000000000001</v>
       </c>
-      <c r="E51" s="6">
+      <c r="E51" s="5">
         <v>5.4</v>
       </c>
-      <c r="F51" s="6">
+      <c r="F51" s="5">
         <v>3.7</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A52" s="5">
+      <c r="A52" s="4">
         <v>44621</v>
       </c>
-      <c r="B52" s="6">
+      <c r="B52" s="5">
         <v>34.5</v>
       </c>
-      <c r="C52" s="6">
+      <c r="C52" s="5">
         <v>39.299999999999997</v>
       </c>
-      <c r="D52" s="6">
+      <c r="D52" s="5">
         <v>17.3</v>
       </c>
-      <c r="E52" s="6">
+      <c r="E52" s="5">
         <v>5.3</v>
       </c>
-      <c r="F52" s="6">
+      <c r="F52" s="5">
         <v>3.6</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A53" s="5">
+      <c r="A53" s="4">
         <v>44652</v>
       </c>
-      <c r="B53" s="6">
+      <c r="B53" s="5">
         <v>34.1</v>
       </c>
-      <c r="C53" s="6">
+      <c r="C53" s="5">
         <v>39.6</v>
       </c>
-      <c r="D53" s="6">
+      <c r="D53" s="5">
         <v>17.399999999999999</v>
       </c>
-      <c r="E53" s="6">
+      <c r="E53" s="5">
         <v>5.2</v>
       </c>
-      <c r="F53" s="6">
+      <c r="F53" s="5">
         <v>3.6</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A54" s="5">
+      <c r="A54" s="4">
         <v>44682</v>
       </c>
-      <c r="B54" s="6">
+      <c r="B54" s="5">
         <v>33.9</v>
       </c>
-      <c r="C54" s="6">
+      <c r="C54" s="5">
         <v>39.6</v>
       </c>
-      <c r="D54" s="6">
+      <c r="D54" s="5">
         <v>17.7</v>
       </c>
-      <c r="E54" s="6">
+      <c r="E54" s="5">
         <v>5.2</v>
       </c>
-      <c r="F54" s="6">
+      <c r="F54" s="5">
         <v>3.6</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A55" s="5">
+      <c r="A55" s="4">
         <v>44713</v>
       </c>
-      <c r="B55" s="6">
+      <c r="B55" s="5">
         <v>33.6</v>
       </c>
-      <c r="C55" s="6">
+      <c r="C55" s="5">
         <v>39.4</v>
       </c>
-      <c r="D55" s="6">
+      <c r="D55" s="5">
         <v>18</v>
       </c>
-      <c r="E55" s="6">
+      <c r="E55" s="5">
         <v>5.4</v>
       </c>
-      <c r="F55" s="6">
+      <c r="F55" s="5">
         <v>3.5</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A56" s="5">
+      <c r="A56" s="4">
         <v>44743</v>
       </c>
-      <c r="B56" s="6">
+      <c r="B56" s="5">
         <v>33.5</v>
       </c>
-      <c r="C56" s="6">
+      <c r="C56" s="5">
         <v>39.200000000000003</v>
       </c>
-      <c r="D56" s="6">
+      <c r="D56" s="5">
         <v>18.100000000000001</v>
       </c>
-      <c r="E56" s="6">
+      <c r="E56" s="5">
         <v>5.6</v>
       </c>
-      <c r="F56" s="6">
+      <c r="F56" s="5">
         <v>3.5</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A57" s="5">
+      <c r="A57" s="4">
         <v>44774</v>
       </c>
-      <c r="B57" s="6">
+      <c r="B57" s="5">
         <v>33.1</v>
       </c>
-      <c r="C57" s="6">
+      <c r="C57" s="5">
         <v>39</v>
       </c>
-      <c r="D57" s="6">
+      <c r="D57" s="5">
         <v>18.399999999999999</v>
       </c>
-      <c r="E57" s="6">
+      <c r="E57" s="5">
         <v>5.8</v>
       </c>
-      <c r="F57" s="6">
+      <c r="F57" s="5">
         <v>3.5</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A58" s="5">
+      <c r="A58" s="4">
         <v>44805</v>
       </c>
-      <c r="B58" s="6">
+      <c r="B58" s="5">
         <v>33.1</v>
       </c>
-      <c r="C58" s="6">
+      <c r="C58" s="5">
         <v>38.799999999999997</v>
       </c>
-      <c r="D58" s="6">
+      <c r="D58" s="5">
         <v>18.600000000000001</v>
       </c>
-      <c r="E58" s="6">
+      <c r="E58" s="5">
         <v>6</v>
       </c>
-      <c r="F58" s="6">
+      <c r="F58" s="5">
         <v>3.5</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A59" s="5">
+      <c r="A59" s="4">
         <v>44835</v>
       </c>
-      <c r="B59" s="6">
+      <c r="B59" s="5">
         <v>33</v>
       </c>
-      <c r="C59" s="6">
+      <c r="C59" s="5">
         <v>38.5</v>
       </c>
-      <c r="D59" s="6">
+      <c r="D59" s="5">
         <v>18.7</v>
       </c>
-      <c r="E59" s="6">
+      <c r="E59" s="5">
         <v>6.2</v>
       </c>
-      <c r="F59" s="6">
+      <c r="F59" s="5">
         <v>3.6</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A60" s="5">
+      <c r="A60" s="4">
         <v>44866</v>
       </c>
-      <c r="B60" s="6">
+      <c r="B60" s="5">
         <v>32.799999999999997</v>
       </c>
-      <c r="C60" s="6">
+      <c r="C60" s="5">
         <v>38.299999999999997</v>
       </c>
-      <c r="D60" s="6">
+      <c r="D60" s="5">
         <v>18.8</v>
       </c>
-      <c r="E60" s="6">
+      <c r="E60" s="5">
         <v>6.4</v>
       </c>
-      <c r="F60" s="6">
+      <c r="F60" s="5">
         <v>3.8</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A61" s="5">
+      <c r="A61" s="4">
         <v>44896</v>
       </c>
-      <c r="B61" s="6">
+      <c r="B61" s="5">
         <v>32.700000000000003</v>
       </c>
-      <c r="C61" s="6">
+      <c r="C61" s="5">
         <v>38.200000000000003</v>
       </c>
-      <c r="D61" s="6">
+      <c r="D61" s="5">
         <v>18.7</v>
       </c>
-      <c r="E61" s="6">
+      <c r="E61" s="5">
         <v>6.5</v>
       </c>
-      <c r="F61" s="6">
+      <c r="F61" s="5">
         <v>3.9</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A62" s="5">
+      <c r="A62" s="4">
         <v>44927</v>
       </c>
-      <c r="B62" s="6">
+      <c r="B62" s="5">
         <v>32.5</v>
       </c>
-      <c r="C62" s="6">
+      <c r="C62" s="5">
         <v>38.1</v>
       </c>
-      <c r="D62" s="6">
+      <c r="D62" s="5">
         <v>18.7</v>
       </c>
-      <c r="E62" s="6">
+      <c r="E62" s="5">
         <v>6.6</v>
       </c>
-      <c r="F62" s="6">
+      <c r="F62" s="5">
         <v>4</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A63" s="5">
+      <c r="A63" s="4">
         <v>44958</v>
       </c>
-      <c r="B63" s="6">
+      <c r="B63" s="5">
         <v>32.4</v>
       </c>
-      <c r="C63" s="6">
+      <c r="C63" s="5">
         <v>38</v>
       </c>
-      <c r="D63" s="6">
+      <c r="D63" s="5">
         <v>18.600000000000001</v>
       </c>
-      <c r="E63" s="6">
+      <c r="E63" s="5">
         <v>6.8</v>
       </c>
-      <c r="F63" s="6">
+      <c r="F63" s="5">
         <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A64" s="5">
+      <c r="A64" s="4">
         <v>44986</v>
       </c>
-      <c r="B64" s="6">
+      <c r="B64" s="5">
         <v>32.299999999999997</v>
       </c>
-      <c r="C64" s="6">
+      <c r="C64" s="5">
         <v>37.799999999999997</v>
       </c>
-      <c r="D64" s="6">
+      <c r="D64" s="5">
         <v>18.600000000000001</v>
       </c>
-      <c r="E64" s="6">
+      <c r="E64" s="5">
         <v>7</v>
       </c>
-      <c r="F64" s="6">
+      <c r="F64" s="5">
         <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A65" s="5">
+      <c r="A65" s="4">
         <v>45017</v>
       </c>
-      <c r="B65" s="6">
+      <c r="B65" s="5">
         <v>32.200000000000003</v>
       </c>
-      <c r="C65" s="6">
+      <c r="C65" s="5">
         <v>37.6</v>
       </c>
-      <c r="D65" s="6">
+      <c r="D65" s="5">
         <v>18.5</v>
       </c>
-      <c r="E65" s="6">
+      <c r="E65" s="5">
         <v>7.2</v>
       </c>
-      <c r="F65" s="6">
+      <c r="F65" s="5">
         <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A66" s="5">
+      <c r="A66" s="4">
         <v>45047</v>
       </c>
-      <c r="B66" s="6">
+      <c r="B66" s="5">
         <v>32</v>
       </c>
-      <c r="C66" s="6">
+      <c r="C66" s="5">
         <v>37.4</v>
       </c>
-      <c r="D66" s="6">
+      <c r="D66" s="5">
         <v>18.399999999999999</v>
       </c>
-      <c r="E66" s="6">
+      <c r="E66" s="5">
         <v>7.4</v>
       </c>
-      <c r="F66" s="6">
+      <c r="F66" s="5">
         <v>4.8</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A67" s="5">
+      <c r="A67" s="4">
         <v>45078</v>
       </c>
-      <c r="B67" s="6">
+      <c r="B67" s="5">
         <v>31.8</v>
       </c>
-      <c r="C67" s="6">
+      <c r="C67" s="5">
         <v>37.1</v>
       </c>
-      <c r="D67" s="6">
+      <c r="D67" s="5">
         <v>18.3</v>
       </c>
-      <c r="E67" s="6">
+      <c r="E67" s="5">
         <v>7.7</v>
       </c>
-      <c r="F67" s="6">
+      <c r="F67" s="5">
         <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A68" s="5">
+      <c r="A68" s="4">
         <v>45108</v>
       </c>
-      <c r="B68" s="6">
+      <c r="B68" s="5">
         <v>31.9</v>
       </c>
-      <c r="C68" s="6">
+      <c r="C68" s="5">
         <v>36.799999999999997</v>
       </c>
-      <c r="D68" s="6">
+      <c r="D68" s="5">
         <v>18</v>
       </c>
-      <c r="E68" s="6">
+      <c r="E68" s="5">
         <v>7.8</v>
       </c>
-      <c r="F68" s="6">
+      <c r="F68" s="5">
         <v>5.5</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A69" s="5">
+      <c r="A69" s="4">
         <v>45139</v>
       </c>
-      <c r="B69" s="6">
+      <c r="B69" s="5">
         <v>32</v>
       </c>
-      <c r="C69" s="6">
+      <c r="C69" s="5">
         <v>36.6</v>
       </c>
-      <c r="D69" s="6">
+      <c r="D69" s="5">
         <v>17.7</v>
       </c>
-      <c r="E69" s="6">
+      <c r="E69" s="5">
         <v>7.8</v>
       </c>
-      <c r="F69" s="6">
+      <c r="F69" s="5">
         <v>5.8</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A70" s="5">
+      <c r="A70" s="4">
         <v>45170</v>
       </c>
-      <c r="B70" s="6">
+      <c r="B70" s="5">
         <v>32.299999999999997</v>
       </c>
-      <c r="C70" s="6">
+      <c r="C70" s="5">
         <v>36.5</v>
       </c>
-      <c r="D70" s="6">
+      <c r="D70" s="5">
         <v>17.5</v>
       </c>
-      <c r="E70" s="6">
+      <c r="E70" s="5">
         <v>7.6</v>
       </c>
-      <c r="F70" s="6">
+      <c r="F70" s="5">
         <v>6.1</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A71" s="5">
+      <c r="A71" s="4">
         <v>45200</v>
       </c>
-      <c r="B71" s="6">
+      <c r="B71" s="5">
         <v>32</v>
       </c>
-      <c r="C71" s="6">
+      <c r="C71" s="5">
         <v>36.299999999999997</v>
       </c>
-      <c r="D71" s="6">
+      <c r="D71" s="5">
         <v>17.399999999999999</v>
       </c>
-      <c r="E71" s="6">
+      <c r="E71" s="5">
         <v>7.6</v>
       </c>
-      <c r="F71" s="6">
+      <c r="F71" s="5">
         <v>6.6</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A72" s="5">
+      <c r="A72" s="4">
         <v>45231</v>
       </c>
-      <c r="B72" s="6">
+      <c r="B72" s="5">
         <v>32.1</v>
       </c>
-      <c r="C72" s="6">
+      <c r="C72" s="5">
         <v>36.200000000000003</v>
       </c>
-      <c r="D72" s="6">
+      <c r="D72" s="5">
         <v>17.2</v>
       </c>
-      <c r="E72" s="6">
+      <c r="E72" s="5">
         <v>7.6</v>
       </c>
-      <c r="F72" s="6">
+      <c r="F72" s="5">
         <v>6.9</v>
       </c>
     </row>
@@ -4445,534 +4455,534 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="8">
+      <c r="A2" s="7">
         <v>43739</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="6">
         <v>100</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="6">
         <v>100</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="6">
         <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="8">
+      <c r="A3" s="7">
         <v>43831</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="6">
         <v>86.657654148431604</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="6">
         <v>76.339062656140698</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="6">
         <v>78.493518479674506</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="8">
+      <c r="A4" s="7">
         <v>43922</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="6">
         <v>1.71734298742066</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="6">
         <v>6.7452783051863696E-2</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="6">
         <v>0.45936988715022897</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="8">
+      <c r="A5" s="7">
         <v>44013</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="6">
         <v>3.2897600989849498</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="6">
         <v>0.154891575896872</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="6">
         <v>1.7430884758988101</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="8">
+      <c r="A6" s="7">
         <v>44105</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="6">
         <v>27.187063217468999</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="6">
         <v>1.0117917457779599</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="6">
         <v>5.4809749549020399</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="8">
+      <c r="A7" s="7">
         <v>44197</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="6">
         <v>48.482574525124299</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="6">
         <v>0.44219046667332901</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="6">
         <v>4.5014053781935699</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="8">
+      <c r="A8" s="7">
         <v>44287</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="6">
         <v>99.500492633411994</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="6">
         <v>0.89187568701908704</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="6">
         <v>11.7443470235348</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="8">
+      <c r="A9" s="7">
         <v>44378</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="6">
         <v>113.915175400408</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="6">
         <v>1.71629859098631</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="6">
         <v>15.742333347317199</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="8">
+      <c r="A10" s="7">
         <v>44470</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="6">
         <v>108.659464289806</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="6">
         <v>2.1984610772459301</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="6">
         <v>27.797122121072299</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="8">
+      <c r="A11" s="7">
         <v>44562</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="6">
         <v>105.21618587173199</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="6">
         <v>2.3283701409013702</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="6">
         <v>44.416243654822303</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="8">
+      <c r="A12" s="7">
         <v>44652</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="6">
         <v>112.593084801686</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="6">
         <v>7.6321574897571702</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="6">
         <v>66.445022444099493</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="8">
+      <c r="A13" s="7">
         <v>44743</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" s="6">
         <v>113.910019934468</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="6">
         <v>17.547716598381101</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="6">
         <v>76.721063892268305</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="8">
+      <c r="A14" s="7">
         <v>44835</v>
       </c>
-      <c r="B14" s="7">
+      <c r="B14" s="6">
         <v>112.021973741493</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="6">
         <v>20.598081343059899</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="6">
         <v>84.039518395771296</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="8">
+      <c r="A15" s="7">
         <v>44927</v>
       </c>
-      <c r="B15" s="7">
+      <c r="B15" s="6">
         <v>112.622299108677</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="6">
         <v>27.932946937143999</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="6">
         <v>89.002391240508402</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="8">
+      <c r="A16" s="7">
         <v>45017</v>
       </c>
-      <c r="B16" s="7">
+      <c r="B16" s="6">
         <v>107.48115390784299</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="6">
         <v>33.7588687918457</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="6">
         <v>86.525149976926599</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="8">
+      <c r="A17" s="7">
         <v>45108</v>
       </c>
-      <c r="B17" s="7">
+      <c r="B17" s="6">
         <v>101.417180303829</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="6">
         <v>36.8317177975417</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="6">
         <v>83.993371649116895</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="8">
+      <c r="A18" s="7">
         <v>45200</v>
       </c>
-      <c r="B18" s="7">
+      <c r="B18" s="6">
         <v>103.865453795569</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="6">
         <v>44.618766863195802</v>
       </c>
-      <c r="D18" s="7">
+      <c r="D18" s="6">
         <v>85.633678734740101</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="8">
+      <c r="A19" s="7">
         <v>45292</v>
       </c>
-      <c r="B19" s="7">
+      <c r="B19" s="6">
         <v>103.852278715945</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C19" s="6">
         <v>43.357149995003503</v>
       </c>
-      <c r="D19" s="7">
+      <c r="D19" s="6">
         <v>85.874900364978799</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="9">
+      <c r="A20" s="8">
         <v>45383</v>
       </c>
-      <c r="B20" s="10">
+      <c r="B20" s="9">
         <v>104.562587356506</v>
       </c>
-      <c r="C20" s="10">
+      <c r="C20" s="9">
         <v>48.3511541920656</v>
       </c>
-      <c r="D20" s="10">
+      <c r="D20" s="9">
         <v>87.240424550069207</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="9">
+      <c r="A21" s="8">
         <v>45474</v>
       </c>
-      <c r="B21" s="10">
+      <c r="B21" s="9">
         <v>106.918635290883</v>
       </c>
-      <c r="C21" s="10">
+      <c r="C21" s="9">
         <v>52.825522134505803</v>
       </c>
-      <c r="D21" s="10">
+      <c r="D21" s="9">
         <v>87.762721819020797</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="9">
+      <c r="A22" s="8">
         <v>45566</v>
       </c>
-      <c r="B22" s="10">
+      <c r="B22" s="9">
         <v>106.114955433861</v>
       </c>
-      <c r="C22" s="10">
+      <c r="C22" s="9">
         <v>54.771659838113301</v>
       </c>
-      <c r="D22" s="10">
+      <c r="D22" s="9">
         <v>88.417166589755396</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="9">
+      <c r="A23" s="8">
         <v>45658</v>
       </c>
-      <c r="B23" s="10">
+      <c r="B23" s="9">
         <v>107.18671951974</v>
       </c>
-      <c r="C23" s="10">
+      <c r="C23" s="9">
         <v>59.4883581492955</v>
       </c>
-      <c r="D23" s="10">
+      <c r="D23" s="9">
         <v>88.954146914460694</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="9">
+      <c r="A24" s="8">
         <v>45748</v>
       </c>
-      <c r="B24" s="10">
+      <c r="B24" s="9">
         <v>107.644983158811</v>
       </c>
-      <c r="C24" s="10">
+      <c r="C24" s="9">
         <v>61.474467872489299</v>
       </c>
-      <c r="D24" s="10">
+      <c r="D24" s="9">
         <v>89.566640097327706</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="9">
+      <c r="A25" s="8">
         <v>45839</v>
       </c>
-      <c r="B25" s="10">
+      <c r="B25" s="9">
         <v>107.52927158994601</v>
       </c>
-      <c r="C25" s="10">
+      <c r="C25" s="9">
         <v>63.5205356250625</v>
       </c>
-      <c r="D25" s="10">
+      <c r="D25" s="9">
         <v>90.174938121407905</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="9">
+      <c r="A26" s="8">
         <v>45931</v>
       </c>
-      <c r="B26" s="10">
+      <c r="B26" s="9">
         <v>108.363311413056</v>
       </c>
-      <c r="C26" s="10">
+      <c r="C26" s="9">
         <v>66.336064754671696</v>
       </c>
-      <c r="D26" s="10">
+      <c r="D26" s="9">
         <v>90.783236145488104</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="9">
+      <c r="A27" s="8">
         <v>46023</v>
       </c>
-      <c r="B27" s="10">
+      <c r="B27" s="9">
         <v>108.566665902894</v>
       </c>
-      <c r="C27" s="10">
+      <c r="C27" s="9">
         <v>67.984910562606203</v>
       </c>
-      <c r="D27" s="10">
+      <c r="D27" s="9">
         <v>91.370558375634502</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="9">
+      <c r="A28" s="8">
         <v>46113</v>
       </c>
-      <c r="B28" s="10">
+      <c r="B28" s="9">
         <v>108.86568292738799</v>
       </c>
-      <c r="C28" s="10">
+      <c r="C28" s="9">
         <v>69.873588488058402</v>
       </c>
-      <c r="D28" s="10">
+      <c r="D28" s="9">
         <v>91.9327096530604</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="9">
+      <c r="A29" s="8">
         <v>46204</v>
       </c>
-      <c r="B29" s="10">
+      <c r="B29" s="9">
         <v>109.404142703297</v>
       </c>
-      <c r="C29" s="10">
+      <c r="C29" s="9">
         <v>71.532427300889395</v>
       </c>
-      <c r="D29" s="10">
+      <c r="D29" s="9">
         <v>92.499056089272997</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="9">
+      <c r="A30" s="8">
         <v>46296</v>
       </c>
-      <c r="B30" s="10">
+      <c r="B30" s="9">
         <v>109.511834658479</v>
       </c>
-      <c r="C30" s="10">
+      <c r="C30" s="9">
         <v>72.746577395822897</v>
       </c>
-      <c r="D30" s="10">
+      <c r="D30" s="9">
         <v>93.065402525485595</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="9">
+      <c r="A31" s="8">
         <v>46388</v>
       </c>
-      <c r="B31" s="10">
+      <c r="B31" s="9">
         <v>109.82631808079201</v>
       </c>
-      <c r="C31" s="10">
+      <c r="C31" s="9">
         <v>74.033176776256596</v>
       </c>
-      <c r="D31" s="10">
+      <c r="D31" s="9">
         <v>93.6212610647313</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="9">
+      <c r="A32" s="8">
         <v>46478</v>
       </c>
-      <c r="B32" s="10">
+      <c r="B32" s="9">
         <v>109.937447013267</v>
       </c>
-      <c r="C32" s="10">
+      <c r="C32" s="9">
         <v>75.052463275706998</v>
       </c>
-      <c r="D32" s="10">
+      <c r="D32" s="9">
         <v>94.089021269455102</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="9">
+      <c r="A33" s="8">
         <v>46569</v>
       </c>
-      <c r="B33" s="10">
+      <c r="B33" s="9">
         <v>109.934582865523</v>
       </c>
-      <c r="C33" s="10">
+      <c r="C33" s="9">
         <v>75.906865194364002</v>
       </c>
-      <c r="D33" s="10">
+      <c r="D33" s="9">
         <v>94.569366950539106</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="9">
+      <c r="A34" s="8">
         <v>46661</v>
       </c>
-      <c r="B34" s="10">
+      <c r="B34" s="9">
         <v>110.09153816190501</v>
       </c>
-      <c r="C34" s="10">
+      <c r="C34" s="9">
         <v>76.723793344658802</v>
       </c>
-      <c r="D34" s="10">
+      <c r="D34" s="9">
         <v>95.039224734656202</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="9">
+      <c r="A35" s="8">
         <v>46753</v>
       </c>
-      <c r="B35" s="10">
+      <c r="B35" s="9">
         <v>110.119033980249</v>
       </c>
-      <c r="C35" s="10">
+      <c r="C35" s="9">
         <v>77.285899870090901</v>
       </c>
-      <c r="D35" s="10">
+      <c r="D35" s="9">
         <v>95.509082518773297</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="9">
+      <c r="A36" s="8">
         <v>46844</v>
       </c>
-      <c r="B36" s="10">
+      <c r="B36" s="9">
         <v>110.168297321449</v>
       </c>
-      <c r="C36" s="10">
+      <c r="C36" s="9">
         <v>77.740581592884993</v>
       </c>
-      <c r="D36" s="10">
+      <c r="D36" s="9">
         <v>95.9726475647103</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="9">
+      <c r="A37" s="8">
         <v>46935</v>
       </c>
-      <c r="B37" s="10">
+      <c r="B37" s="9">
         <v>110.266251174301</v>
       </c>
-      <c r="C37" s="10">
+      <c r="C37" s="9">
         <v>78.117817527730594</v>
       </c>
-      <c r="D37" s="10">
+      <c r="D37" s="9">
         <v>96.434115031253896</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="9">
+      <c r="A38" s="8">
         <v>47027</v>
       </c>
-      <c r="B38" s="10">
+      <c r="B38" s="9">
         <v>110.28343606076599</v>
       </c>
-      <c r="C38" s="10">
+      <c r="C38" s="9">
         <v>78.382632157489795</v>
       </c>
-      <c r="D38" s="10">
+      <c r="D38" s="9">
         <v>96.893484918404198</v>
       </c>
     </row>
@@ -4992,57 +5002,57 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="12">
+      <c r="B2" s="11">
         <v>1392.1120000000001</v>
       </c>
-      <c r="C2" s="12">
+      <c r="C2" s="11">
         <v>1276.4010000000001</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="11">
         <v>57.374000000000002</v>
       </c>
-      <c r="C3" s="11">
+      <c r="C3" s="10">
         <v>87.100999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="11">
         <v>91.119</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="11">
         <v>84.71</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="11">
         <v>216.87899999999999</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="11">
         <v>249.46700000000001</v>
       </c>
     </row>
@@ -5055,220 +5065,234 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F07ED02-34FA-BF43-9616-CD6DB370A5A2}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="6">
+      <c r="A2" s="5">
         <v>2010</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="5">
         <v>8984</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="5">
         <v>8166</v>
       </c>
-      <c r="D2" s="6">
-        <v>4.6898080000000002</v>
+      <c r="D2" s="5">
+        <f xml:space="preserve"> 4.689808 / 100</f>
+        <v>4.6898080000000002E-2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="6">
+      <c r="A3" s="5">
         <v>2011</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="5">
         <v>8285</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="5">
         <v>7336</v>
       </c>
-      <c r="D3" s="6">
-        <v>4.4478850000000003</v>
+      <c r="D3" s="5">
+        <f>4.447885 / 100</f>
+        <v>4.447885E-2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="6">
+      <c r="A4" s="5">
         <v>2012</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="5">
         <v>7194</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <v>6839</v>
       </c>
-      <c r="D4" s="6">
-        <v>3.6575000000000002</v>
+      <c r="D4" s="5">
+        <f xml:space="preserve"> 3.6575 / 100</f>
+        <v>3.6575000000000003E-2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="6">
+      <c r="A5" s="5">
         <v>2013</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <v>7704</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>7227</v>
       </c>
-      <c r="D5" s="6">
-        <v>3.9755769999999999</v>
+      <c r="D5" s="5">
+        <f xml:space="preserve"> 3.975577 / 100</f>
+        <v>3.9755769999999996E-2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="6">
+      <c r="A6" s="5">
         <v>2014</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="5">
         <v>9669</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <v>8382</v>
       </c>
-      <c r="D6" s="6">
-        <v>4.1688679999999998</v>
+      <c r="D6" s="5">
+        <f xml:space="preserve"> 4.168868 / 100</f>
+        <v>4.1688679999999999E-2</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="6">
+      <c r="A7" s="5">
         <v>2015</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="5">
         <v>9847</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <v>7822</v>
       </c>
-      <c r="D7" s="6">
-        <v>3.8505769999999999</v>
+      <c r="D7" s="5">
+        <f xml:space="preserve"> 3.850577 / 100</f>
+        <v>3.8505770000000002E-2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="6">
+      <c r="A8" s="5">
         <v>2016</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="5">
         <v>9798</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="5">
         <v>8038</v>
       </c>
-      <c r="D8" s="6">
-        <v>3.6540379999999999</v>
+      <c r="D8" s="5">
+        <f xml:space="preserve"> 3.654038/100</f>
+        <v>3.6540379999999997E-2</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="6">
+      <c r="A9" s="5">
         <v>2017</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="5">
         <v>10703</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <v>10552</v>
       </c>
-      <c r="D9" s="6">
-        <v>3.989808</v>
+      <c r="D9" s="5">
+        <f xml:space="preserve"> 3.989808 / 100</f>
+        <v>3.9898080000000002E-2</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="6">
+      <c r="A10" s="5">
         <v>2018</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="5">
         <v>8220</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="5">
         <v>6177</v>
       </c>
-      <c r="D10" s="6">
-        <v>4.5446150000000003</v>
+      <c r="D10" s="5">
+        <f>4.544615/100</f>
+        <v>4.5446150000000005E-2</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="6">
+      <c r="A11" s="5">
         <v>2019</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="5">
         <v>9235</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="5">
         <v>7954</v>
       </c>
-      <c r="D11" s="6">
-        <v>3.9357690000000001</v>
+      <c r="D11" s="5">
+        <f>3.935769/100</f>
+        <v>3.9357690000000001E-2</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="6">
+      <c r="A12" s="5">
         <v>2020</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="5">
         <v>9577</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="5">
         <v>9110</v>
       </c>
-      <c r="D12" s="6">
-        <v>3.1116980000000001</v>
+      <c r="D12" s="5">
+        <f>3.111698/100</f>
+        <v>3.1116980000000002E-2</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="6">
+      <c r="A13" s="5">
         <v>2021</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="5">
         <v>14722</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="5">
         <v>11493</v>
       </c>
-      <c r="D13" s="6">
-        <v>2.9576920000000002</v>
+      <c r="D13" s="5">
+        <f>2.957692/100</f>
+        <v>2.9576920000000003E-2</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="6">
+      <c r="A14" s="5">
         <v>2022</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="5">
         <v>11408</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="5">
         <v>8894</v>
       </c>
-      <c r="D14" s="6">
-        <v>5.3440380000000003</v>
+      <c r="D14" s="5">
+        <f>5.344038/100</f>
+        <v>5.3440380000000003E-2</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="6">
+      <c r="A15" s="5">
         <v>2023</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="5">
         <v>7337</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="5">
         <v>5636</v>
       </c>
-      <c r="D15" s="6">
-        <v>6.8304</v>
+      <c r="D15" s="5">
+        <f>6.8304/100</f>
+        <v>6.8304000000000004E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add support for Trillion units
</commit_message>
<xml_diff>
--- a/sample_data/SampleData.xlsx
+++ b/sample_data/SampleData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vicky/Documents/R/UHEROtheme/sample_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16D638C4-FABF-DD4B-9FD4-06BF39F005FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A99A23FE-BB5C-0A4D-AD8E-C7B4FF7D9C42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6360" yWindow="1700" windowWidth="27240" windowHeight="16440" activeTab="1" xr2:uid="{37EF705C-9ABB-BC49-956B-53E83ECDB111}"/>
+    <workbookView xWindow="4620" yWindow="1100" windowWidth="27240" windowHeight="16440" activeTab="7" xr2:uid="{37EF705C-9ABB-BC49-956B-53E83ECDB111}"/>
   </bookViews>
   <sheets>
     <sheet name="Nonfarm Payrolls" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Vis by Market Forecast" sheetId="5" r:id="rId5"/>
     <sheet name="Vexp By Mkt" sheetId="6" r:id="rId6"/>
     <sheet name="Transactions" sheetId="8" r:id="rId7"/>
+    <sheet name="IncomeEquities" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
   <si>
     <t>Date</t>
   </si>
@@ -166,6 +167,12 @@
   <si>
     <t>Interest Rate</t>
   </si>
+  <si>
+    <t>Disposable Personal Income</t>
+  </si>
+  <si>
+    <t>Corporate Equities &amp; Mutual Fund Shares</t>
+  </si>
 </sst>
 </file>
 
@@ -174,7 +181,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -214,6 +221,25 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -245,7 +271,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -258,6 +284,10 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="11" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1633,7 +1663,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A79EC09-1951-2A4F-9892-1CD1D59E1A18}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
@@ -5298,4 +5328,140 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC7B0A04-130F-334A-ACDD-FC0CA98C746F}">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="14">
+        <v>44927</v>
+      </c>
+      <c r="B2" s="15">
+        <v>20283400000000</v>
+      </c>
+      <c r="C2" s="15">
+        <v>36520700000000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="14">
+        <v>45017</v>
+      </c>
+      <c r="B3" s="15">
+        <v>20651000000000</v>
+      </c>
+      <c r="C3" s="15">
+        <v>38627200000000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="14">
+        <v>45108</v>
+      </c>
+      <c r="B4" s="15">
+        <v>20894600000000</v>
+      </c>
+      <c r="C4" s="15">
+        <v>37204700000000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="14">
+        <v>45200</v>
+      </c>
+      <c r="B5" s="15">
+        <v>21168000000000</v>
+      </c>
+      <c r="C5" s="15">
+        <v>40738200000000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="14">
+        <v>45292</v>
+      </c>
+      <c r="B6" s="15">
+        <v>21575400000000</v>
+      </c>
+      <c r="C6" s="15">
+        <v>44267800000000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="14">
+        <v>45383</v>
+      </c>
+      <c r="B7" s="15">
+        <v>21843200000000</v>
+      </c>
+      <c r="C7" s="15">
+        <v>45057300000000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="14">
+        <v>45474</v>
+      </c>
+      <c r="B8" s="15">
+        <v>22002600000000</v>
+      </c>
+      <c r="C8" s="15">
+        <v>48147900000000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="14">
+        <v>45566</v>
+      </c>
+      <c r="B9" s="15">
+        <v>22249500000000</v>
+      </c>
+      <c r="C9" s="15">
+        <v>48547800000000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="14">
+        <v>45658</v>
+      </c>
+      <c r="B10" s="15">
+        <v>22563700000000</v>
+      </c>
+      <c r="C10" s="15">
+        <v>46723700000000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="14">
+        <v>45748</v>
+      </c>
+      <c r="B11" s="15">
+        <v>22858500000000</v>
+      </c>
+      <c r="C11" s="15">
+        <v>51186500000000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>